<commit_message>
Replace with 2021-0294105 files
</commit_message>
<xml_diff>
--- a/2021-0294106_digestate_acidification/inputs/inputs.xlsx
+++ b/2021-0294106_digestate_acidification/inputs/inputs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Slurry" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="37">
   <si>
     <t xml:space="preserve">man.name</t>
   </si>
@@ -30,6 +30,9 @@
     <t xml:space="preserve">man.source</t>
   </si>
   <si>
+    <t xml:space="preserve">acid</t>
+  </si>
+  <si>
     <t xml:space="preserve">man.dm</t>
   </si>
   <si>
@@ -39,19 +42,25 @@
     <t xml:space="preserve">Svinegylle</t>
   </si>
   <si>
-    <t xml:space="preserve">pig</t>
+    <t xml:space="preserve">Pig</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FALSE</t>
   </si>
   <si>
     <t xml:space="preserve">Kvæggylle</t>
   </si>
   <si>
-    <t xml:space="preserve">cattle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Agfasset biomasse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">digestate</t>
+    <t xml:space="preserve">Cattle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Afgasset biomasse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Digestate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRUE</t>
   </si>
   <si>
     <t xml:space="preserve">app.timing.dk</t>
@@ -108,20 +117,34 @@
     <t xml:space="preserve">app.rate.ni</t>
   </si>
   <si>
-    <t xml:space="preserve">bsth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">none</t>
+    <t xml:space="preserve">Trailing hose</t>
+  </si>
+  <si>
+    <t xml:space="preserve">None</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shallow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deep</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Open slot injection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Closed slot injection</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="@"/>
+    <numFmt numFmtId="166" formatCode="0.00"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -143,6 +166,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF3465A4"/>
+      <name val="Sans"/>
+      <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -187,7 +217,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -196,7 +226,15 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -209,6 +247,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF3465A4"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -217,17 +315,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.08203125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.22"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="3" style="1" width="10.08"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="10.08"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="4" style="1" width="10.08"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -237,72 +336,120 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1" t="n">
         <v>3.9</v>
       </c>
-      <c r="D2" s="1" t="n">
+      <c r="E2" s="3" t="n">
         <v>7.2</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1" t="n">
+      <c r="D3" s="1" t="n">
         <v>6.5</v>
       </c>
-      <c r="D3" s="1" t="n">
+      <c r="E3" s="3" t="n">
         <v>7</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>5.1</v>
+      </c>
+      <c r="E4" s="3" t="n">
+        <v>7.9</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>3.9</v>
+      </c>
+      <c r="E5" s="4" t="n">
+        <f aca="false">E2-0.73</f>
+        <v>6.47</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="1" t="n">
+      <c r="C6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="E6" s="4" t="n">
+        <f aca="false">E3-0.53</f>
+        <v>6.47</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="1" t="n">
         <v>5.1</v>
       </c>
-      <c r="D4" s="1" t="n">
-        <v>7.9</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
+      <c r="E7" s="4" t="n">
+        <f aca="false">E4-1.38</f>
+        <v>6.52</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -322,8 +469,8 @@
   </sheetPr>
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.08203125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -338,27 +485,27 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>4.9</v>
@@ -372,10 +519,10 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>8.5</v>
@@ -389,10 +536,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>12.4</v>
@@ -406,10 +553,10 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>16.867</v>
@@ -423,10 +570,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C6" s="1" t="n">
         <v>14.6</v>
@@ -454,47 +601,93 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.08203125" defaultRowHeight="14.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="1" style="1" width="10.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.3"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="2" style="1" width="10.08"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>30</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Apply to digestate questions
</commit_message>
<xml_diff>
--- a/2021-0294106_digestate_acidification/inputs/inputs.xlsx
+++ b/2021-0294106_digestate_acidification/inputs/inputs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Slurry" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
   <si>
     <t xml:space="preserve">man.name</t>
   </si>
@@ -39,28 +39,19 @@
     <t xml:space="preserve">man.ph</t>
   </si>
   <si>
-    <t xml:space="preserve">Svinegylle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pig</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FALSE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kvæggylle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cattle</t>
-  </si>
-  <si>
     <t xml:space="preserve">Afgasset biomasse</t>
   </si>
   <si>
     <t xml:space="preserve">Digestate</t>
   </si>
   <si>
-    <t xml:space="preserve">TRUE</t>
+    <t xml:space="preserve">0 kg/t</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11 kg/t</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.1 kg/t</t>
   </si>
   <si>
     <t xml:space="preserve">app.timing.dk</t>
@@ -108,25 +99,10 @@
     <t xml:space="preserve">app.mthd</t>
   </si>
   <si>
-    <t xml:space="preserve">incorp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">t.incorp</t>
-  </si>
-  <si>
     <t xml:space="preserve">app.rate.ni</t>
   </si>
   <si>
     <t xml:space="preserve">Trailing hose</t>
-  </si>
-  <si>
-    <t xml:space="preserve">None</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shallow</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Deep</t>
   </si>
   <si>
     <t xml:space="preserve">Open slot injection</t>
@@ -315,15 +291,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.08203125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="18.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.22"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="10.08"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="4" style="1" width="10.08"/>
@@ -357,98 +333,46 @@
         <v>7</v>
       </c>
       <c r="D2" s="1" t="n">
-        <v>3.9</v>
+        <v>5.1</v>
       </c>
       <c r="E2" s="3" t="n">
-        <v>7.2</v>
+        <v>7.9</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="D3" s="1" t="n">
-        <v>6.5</v>
-      </c>
-      <c r="E3" s="3" t="n">
-        <v>7</v>
+        <v>5.1</v>
+      </c>
+      <c r="E3" s="4" t="n">
+        <f aca="false">7.9-1.38</f>
+        <v>6.52</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>5.1</v>
       </c>
-      <c r="E4" s="3" t="n">
-        <v>7.9</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="1" t="n">
-        <v>3.9</v>
-      </c>
-      <c r="E5" s="4" t="n">
-        <f aca="false">E2-0.73</f>
-        <v>6.47</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="1" t="n">
-        <v>6.5</v>
-      </c>
-      <c r="E6" s="4" t="n">
-        <f aca="false">E3-0.53</f>
-        <v>6.47</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="1" t="n">
-        <v>5.1</v>
-      </c>
-      <c r="E7" s="4" t="n">
-        <f aca="false">E4-1.38</f>
-        <v>6.52</v>
+      <c r="E4" s="4" t="n">
+        <f aca="false">7.9-0.583</f>
+        <v>7.317</v>
       </c>
     </row>
   </sheetData>
@@ -485,27 +409,27 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>4.9</v>
@@ -519,10 +443,10 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>8.5</v>
@@ -536,10 +460,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>12.4</v>
@@ -553,10 +477,10 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>16.867</v>
@@ -570,10 +494,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C6" s="1" t="n">
         <v>14.6</v>
@@ -601,90 +525,47 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.08203125" defaultRowHeight="14.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.08203125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.3"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="2" style="1" width="10.08"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1021" min="2" style="1" width="10.08"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B2" s="1" t="n">
         <v>30</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="D3" s="1" t="n">
-        <v>30</v>
+        <v>27</v>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C4" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="D4" s="1" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D5" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B4" s="1" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add additional intermediate acid dose.
Add 5.7 kg/t for updated 25% reduction relative to un-treated digestate.
</commit_message>
<xml_diff>
--- a/2021-0294106_digestate_acidification/inputs/inputs.xlsx
+++ b/2021-0294106_digestate_acidification/inputs/inputs.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="30">
   <si>
     <t xml:space="preserve">man.name</t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t xml:space="preserve">2.1 kg/t</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.7 kg/t</t>
   </si>
   <si>
     <t xml:space="preserve">app.timing.dk</t>
@@ -291,10 +294,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.08203125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -373,6 +376,24 @@
       <c r="E4" s="4" t="n">
         <f aca="false">7.9-0.583</f>
         <v>7.317</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>5.1</v>
+      </c>
+      <c r="E5" s="4" t="n">
+        <f aca="false">7.9-1.01</f>
+        <v>6.89</v>
       </c>
     </row>
   </sheetData>
@@ -409,27 +430,27 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>4.9</v>
@@ -443,10 +464,10 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>8.5</v>
@@ -460,10 +481,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>12.4</v>
@@ -477,10 +498,10 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>16.867</v>
@@ -494,10 +515,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C6" s="1" t="n">
         <v>14.6</v>
@@ -539,15 +560,15 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>30</v>
@@ -555,7 +576,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>0</v>
@@ -563,7 +584,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Switch to use new prep = TRUE option, add EF table
</commit_message>
<xml_diff>
--- a/2021-0294106_digestate_acidification/inputs/inputs.xlsx
+++ b/2021-0294106_digestate_acidification/inputs/inputs.xlsx
@@ -22,10 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="30">
-  <si>
-    <t xml:space="preserve">man.name</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
   <si>
     <t xml:space="preserve">man.source</t>
   </si>
@@ -40,9 +37,6 @@
   </si>
   <si>
     <t xml:space="preserve">Afgasset biomasse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Digestate</t>
   </si>
   <si>
     <t xml:space="preserve">0 kg/t</t>
@@ -294,104 +288,88 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
+      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.08203125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="18.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.22"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="10.08"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="4" style="1" width="10.08"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="10.08"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="3" style="1" width="10.08"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="1" t="n">
+      <c r="C2" s="1" t="n">
         <v>5.1</v>
       </c>
-      <c r="E2" s="3" t="n">
+      <c r="D2" s="3" t="n">
         <v>7.9</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="1" t="n">
+      <c r="C3" s="1" t="n">
         <v>5.1</v>
       </c>
-      <c r="E3" s="4" t="n">
+      <c r="D3" s="4" t="n">
         <f aca="false">7.9-1.38</f>
         <v>6.52</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="1" t="n">
         <v>5.1</v>
       </c>
-      <c r="E4" s="4" t="n">
+      <c r="D4" s="4" t="n">
         <f aca="false">7.9-0.583</f>
         <v>7.317</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="1" t="n">
         <v>5.1</v>
       </c>
-      <c r="E5" s="4" t="n">
+      <c r="D5" s="4" t="n">
         <f aca="false">7.9-1.01</f>
         <v>6.89</v>
       </c>
@@ -430,27 +408,27 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>4.9</v>
@@ -464,10 +442,10 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>8.5</v>
@@ -481,10 +459,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>12.4</v>
@@ -498,10 +476,10 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>16.867</v>
@@ -515,10 +493,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C6" s="1" t="n">
         <v>14.6</v>
@@ -560,15 +538,15 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>30</v>
@@ -576,7 +554,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>0</v>
@@ -584,7 +562,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>0</v>

</xml_diff>